<commit_message>
Exported gerbers finished everything off. REV A
</commit_message>
<xml_diff>
--- a/MITAvionics/Hours.xlsx
+++ b/MITAvionics/Hours.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>Time H/M/S</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>Layout work</t>
+  </si>
+  <si>
+    <t>everything else</t>
   </si>
 </sst>
 </file>
@@ -355,10 +358,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E8"/>
+  <dimension ref="B3:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -431,6 +434,17 @@
         <v>3</v>
       </c>
     </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B9" s="1">
+        <v>42160</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
finished adding hours to invoice
</commit_message>
<xml_diff>
--- a/MITAvionics/Hours.xlsx
+++ b/MITAvionics/Hours.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="7820" windowHeight="5000"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="7820" windowHeight="5000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>Time H/M/S</t>
   </si>
@@ -42,14 +42,76 @@
   </si>
   <si>
     <t>assembly</t>
+  </si>
+  <si>
+    <t>shipping cost</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>Rate($/hr)</t>
+  </si>
+  <si>
+    <t>pcb layout work</t>
+  </si>
+  <si>
+    <t>pcb Layout work</t>
+  </si>
+  <si>
+    <t>Other expenses</t>
+  </si>
+  <si>
+    <t>Hourly work</t>
+  </si>
+  <si>
+    <t>single day shipping</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Rebtes</t>
+  </si>
+  <si>
+    <t>Friends and family discount</t>
+  </si>
+  <si>
+    <t>2 for 20 discount</t>
+  </si>
+  <si>
+    <t>Hourly total</t>
+  </si>
+  <si>
+    <t>other expenses total</t>
+  </si>
+  <si>
+    <t>rebates total</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -77,11 +139,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,17 +428,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E10"/>
+  <dimension ref="A3:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.453125" customWidth="1"/>
+    <col min="1" max="1" width="16.90625" customWidth="1"/>
+    <col min="2" max="2" width="23.6328125" customWidth="1"/>
     <col min="3" max="3" width="11.90625" customWidth="1"/>
-    <col min="5" max="5" width="15.453125" customWidth="1"/>
+    <col min="4" max="4" width="11.26953125" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" customWidth="1"/>
+    <col min="6" max="6" width="17.6328125" customWidth="1"/>
+    <col min="7" max="7" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.35">
@@ -460,7 +530,274 @@
         <v>5</v>
       </c>
     </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C11" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C12" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D14">
+        <v>66.64</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.11851851851851852</v>
+      </c>
+      <c r="D21">
+        <v>15</v>
+      </c>
+      <c r="E21">
+        <f>((C21-INT(C21))*24)*D21</f>
+        <v>42.666666666666671</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D22">
+        <v>15</v>
+      </c>
+      <c r="E22">
+        <f t="shared" ref="E22:E29" si="0">((C22-INT(C22))*24)*D22</f>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="2">
+        <v>2.2222222222222223E-2</v>
+      </c>
+      <c r="D23">
+        <v>15</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="2">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D24">
+        <v>15</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.3125</v>
+      </c>
+      <c r="D25">
+        <v>15</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>112.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D26">
+        <v>15</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="3">
+        <v>9.0277777777777776E-2</v>
+      </c>
+      <c r="D27">
+        <v>15</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="D28">
+        <v>15</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D29">
+        <v>15</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F30" t="s">
+        <v>20</v>
+      </c>
+      <c r="G30">
+        <f>SUM(E21:E29)</f>
+        <v>555.66666666666674</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32">
+        <v>66.64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F33" t="s">
+        <v>21</v>
+      </c>
+      <c r="G33">
+        <f>SUM(E32)</f>
+        <v>66.64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35">
+        <v>-150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36">
+        <v>-172.30600000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G37">
+        <f>SUM(E35:E36)</f>
+        <v>-322.30600000000004</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F41" t="s">
+        <v>23</v>
+      </c>
+      <c r="G41">
+        <f>SUM(G30,G33,G37)</f>
+        <v>300.00066666666669</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>